<commit_message>
Refactor Excel export logic to utilize template and update package handling in marks
</commit_message>
<xml_diff>
--- a/templates/f10_template.xlsx
+++ b/templates/f10_template.xlsx
@@ -184,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -445,6 +445,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -563,7 +578,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1100,7 +1115,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
+      <selection pane="bottomRight" activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1109,19 +1124,8 @@
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="4" width="11.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="5.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6" style="1" customWidth="1"/>
-    <col min="9" max="13" width="5.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.28515625" style="1" customWidth="1"/>
-    <col min="18" max="19" width="5.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="5.7109375" style="1" customWidth="1"/>
-    <col min="25" max="27" width="6.5703125" style="1" customWidth="1"/>
-    <col min="28" max="29" width="5.7109375" style="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" customWidth="1"/>
+    <col min="6" max="29" width="5.7109375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" style="1" customWidth="1"/>
     <col min="31" max="31" width="5.7109375" style="1" customWidth="1"/>
     <col min="32" max="16384" width="11.5703125" style="1"/>
   </cols>

</xml_diff>